<commit_message>
Bulk Mails On Imported Lecs Via XLS
</commit_message>
<xml_diff>
--- a/public/templates/ezanaLMS_Lecturers_XLS_Template.xlsx
+++ b/public/templates/ezanaLMS_Lecturers_XLS_Template.xlsx
@@ -52,7 +52,7 @@
     <t xml:space="preserve">Employee ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Date Employes</t>
+    <t xml:space="preserve">Date Employed (MM/DD/YYYY)</t>
   </si>
   <si>
     <t xml:space="preserve">Lecturer Status (Either On Work Or On Leave)</t>
@@ -62,14 +62,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -91,6 +93,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,12 +145,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -161,24 +179,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="19.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="33.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="34.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="42.79"/>
   </cols>
   <sheetData>
@@ -219,6 +237,96 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K21" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>